<commit_message>
Organisation of folder and code, Structure document for disso
</commit_message>
<xml_diff>
--- a/Research/Diagrams/Stats.xlsx
+++ b/Research/Diagrams/Stats.xlsx
@@ -319,16 +319,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8028</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3537</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -476,16 +476,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67</c:v>
+                  <c:v>7998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>3530</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -633,16 +633,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>98</c:v>
+                  <c:v>5515</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>2303</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>1298</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -790,16 +790,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>3437</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1145,16 +1145,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8028</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98</c:v>
+                  <c:v>3537</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1273,16 +1273,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>7998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>3530</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1401,16 +1401,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5515</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>2303</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>1298</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1529,16 +1529,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>3437</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>3601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1959,16 +1959,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8028</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98</c:v>
+                  <c:v>3537</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2322,16 +2322,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>7998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>3530</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2685,16 +2685,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5515</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>2303</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>1298</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3048,16 +3048,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>3437</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>3601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6994,8 +6994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7025,16 +7025,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>8028</v>
       </c>
       <c r="C2">
-        <v>67</v>
+        <v>7998</v>
       </c>
       <c r="D2">
-        <v>98</v>
+        <v>5515</v>
       </c>
       <c r="E2">
-        <v>65</v>
+        <v>3437</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -7042,16 +7042,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="D3">
-        <v>13</v>
+        <v>2303</v>
       </c>
       <c r="E3">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7059,16 +7059,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>3537</v>
       </c>
       <c r="C4">
-        <v>32</v>
+        <v>3530</v>
       </c>
       <c r="D4">
-        <v>54</v>
+        <v>1298</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -7076,16 +7076,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C5">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D5">
-        <v>23</v>
+        <v>961</v>
       </c>
       <c r="E5">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7099,8 +7099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7130,16 +7130,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>8028</v>
       </c>
       <c r="C2">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2">
-        <v>98</v>
+        <v>3537</v>
       </c>
       <c r="E2">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -7147,16 +7147,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>7998</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="D3">
-        <v>13</v>
+        <v>3530</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -7164,16 +7164,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5515</v>
       </c>
       <c r="C4">
-        <v>32</v>
+        <v>2303</v>
       </c>
       <c r="D4">
-        <v>54</v>
+        <v>1298</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>961</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -7181,16 +7181,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>3437</v>
       </c>
       <c r="C5">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>23</v>
+        <v>3601</v>
       </c>
       <c r="E5">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>